<commit_message>
before implement view table
</commit_message>
<xml_diff>
--- a/data/call/callReason.xlsx
+++ b/data/call/callReason.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\C&amp;S Data Pipeline\Processed data\call\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5126C15C-1E8C-4CB0-A62F-40A2895F494B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CABA57D8-6D24-404F-A015-E36AE3CCF03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3180" yWindow="6120" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="callReason" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>callReason</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>ابلاغ</t>
+  </si>
+  <si>
+    <t>متابعة طلب صيانة</t>
+  </si>
+  <si>
+    <t>متابعه شكوى</t>
   </si>
 </sst>
 </file>
@@ -543,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -842,7 +848,40 @@
         <v>35</v>
       </c>
     </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>